<commit_message>
AE, EG, SC changed to normalized/denormalized layout. Additional collection groups for EG included
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_AE.xlsx
+++ b/curation/draft/collection/collection_specialization_AE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27CA50D-4DDD-4EBA-A865-8AC7569FCBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353760AE-C760-7D46-B5D1-4C63A954E0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="6640" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_AE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_AE!$A$1:$AG$34</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="135">
   <si>
     <t>package_date</t>
   </si>
@@ -332,9 +332,6 @@
     <t>CDASHIG</t>
   </si>
   <si>
-    <t>Vertical</t>
-  </si>
-  <si>
     <t>Single</t>
   </si>
   <si>
@@ -344,24 +341,9 @@
     <t>No;Yes</t>
   </si>
   <si>
-    <t>AE_VERTICAL</t>
-  </si>
-  <si>
     <t>2-1</t>
   </si>
   <si>
-    <t>AE_HORIZONTAL</t>
-  </si>
-  <si>
-    <t>Horizontal</t>
-  </si>
-  <si>
-    <t>Adverse Event Free Text Format (Vertical)</t>
-  </si>
-  <si>
-    <t>Adverse Event Free Text Format (Horizontal)</t>
-  </si>
-  <si>
     <t>[NOT SUBMITTED]</t>
   </si>
   <si>
@@ -441,6 +423,24 @@
   </si>
   <si>
     <t>[NOT SUBMITTED];AEENRTPT; AEENRF</t>
+  </si>
+  <si>
+    <t>AE_DENORMALIZED</t>
+  </si>
+  <si>
+    <t>Denormalized</t>
+  </si>
+  <si>
+    <t>Adverse Event Free Text Format (Denormalized)</t>
+  </si>
+  <si>
+    <t>AE_NORMALIZED</t>
+  </si>
+  <si>
+    <t>Normalized</t>
+  </si>
+  <si>
+    <t>Adverse Event Free Text Format (Normalized)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -541,6 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,42 +846,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AS1" sqref="AS1"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="23.83203125" style="3" customWidth="1"/>
     <col min="16" max="16" width="27" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" customWidth="1"/>
-    <col min="24" max="24" width="30.85546875" customWidth="1"/>
-    <col min="25" max="25" width="21.28515625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="22.7109375" style="3" customWidth="1"/>
-    <col min="27" max="27" width="19.42578125" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" customWidth="1"/>
-    <col min="29" max="29" width="14.7109375" customWidth="1"/>
-    <col min="30" max="30" width="18.85546875" customWidth="1"/>
-    <col min="31" max="31" width="16.85546875" customWidth="1"/>
-    <col min="32" max="32" width="15.42578125" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" customWidth="1"/>
+    <col min="20" max="20" width="12.5" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" customWidth="1"/>
+    <col min="24" max="24" width="30.83203125" customWidth="1"/>
+    <col min="25" max="25" width="21.33203125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="22.6640625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="19.5" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" customWidth="1"/>
+    <col min="29" max="29" width="14.6640625" customWidth="1"/>
+    <col min="30" max="30" width="18.83203125" customWidth="1"/>
+    <col min="31" max="31" width="16.83203125" customWidth="1"/>
+    <col min="32" max="32" width="15.5" customWidth="1"/>
+    <col min="33" max="33" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -981,15 +982,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
         <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
@@ -998,7 +999,7 @@
         <v>33</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L2" t="s">
         <v>46</v>
@@ -1007,7 +1008,7 @@
         <v>46</v>
       </c>
       <c r="N2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>47</v>
@@ -1028,22 +1029,22 @@
         <v>59</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AE2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -1054,19 +1055,19 @@
         <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L3" t="s">
         <v>34</v>
@@ -1099,7 +1100,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -1110,19 +1111,19 @@
         <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
-        <v>102</v>
+      <c r="H4" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L4" t="s">
         <v>49</v>
@@ -1131,7 +1132,7 @@
         <v>49</v>
       </c>
       <c r="N4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>50</v>
@@ -1155,7 +1156,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -1166,19 +1167,19 @@
         <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
-        <v>102</v>
+      <c r="H5" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L5" t="s">
         <v>52</v>
@@ -1187,7 +1188,7 @@
         <v>52</v>
       </c>
       <c r="N5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>53</v>
@@ -1208,19 +1209,19 @@
         <v>48</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -1231,19 +1232,19 @@
         <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" t="s">
-        <v>102</v>
+      <c r="H6" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L6" t="s">
         <v>54</v>
@@ -1252,7 +1253,7 @@
         <v>54</v>
       </c>
       <c r="N6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>55</v>
@@ -1276,7 +1277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -1287,19 +1288,19 @@
         <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
-        <v>102</v>
+      <c r="H7" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I7" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L7" t="s">
         <v>39</v>
@@ -1338,7 +1339,7 @@
         <v>45</v>
       </c>
       <c r="AA7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD7" t="s">
         <v>39</v>
@@ -1347,7 +1348,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -1358,19 +1359,19 @@
         <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="H8" t="s">
-        <v>102</v>
+      <c r="H8" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L8" t="s">
         <v>56</v>
@@ -1400,16 +1401,16 @@
         <v>59</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y8" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD8" t="s">
         <v>56</v>
@@ -1418,7 +1419,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>32</v>
       </c>
@@ -1429,19 +1430,19 @@
         <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="H9" t="s">
-        <v>102</v>
+      <c r="H9" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L9" t="s">
         <v>60</v>
@@ -1471,16 +1472,16 @@
         <v>59</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y9" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD9" t="s">
         <v>60</v>
@@ -1489,7 +1490,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -1500,19 +1501,19 @@
         <v>97</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" t="s">
-        <v>102</v>
+      <c r="H10" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I10" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L10" t="s">
         <v>63</v>
@@ -1542,16 +1543,16 @@
         <v>59</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y10" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD10" t="s">
         <v>63</v>
@@ -1560,7 +1561,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -1571,19 +1572,19 @@
         <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
         <v>33</v>
       </c>
-      <c r="H11" t="s">
-        <v>102</v>
+      <c r="H11" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I11" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L11" t="s">
         <v>66</v>
@@ -1613,16 +1614,16 @@
         <v>59</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y11" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD11" t="s">
         <v>66</v>
@@ -1631,7 +1632,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1642,19 +1643,19 @@
         <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
         <v>33</v>
       </c>
-      <c r="H12" t="s">
-        <v>102</v>
+      <c r="H12" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L12" t="s">
         <v>69</v>
@@ -1684,16 +1685,16 @@
         <v>59</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y12" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD12" t="s">
         <v>69</v>
@@ -1702,7 +1703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -1713,19 +1714,19 @@
         <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G13" t="s">
         <v>33</v>
       </c>
-      <c r="H13" t="s">
-        <v>102</v>
+      <c r="H13" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I13" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L13" t="s">
         <v>72</v>
@@ -1755,16 +1756,16 @@
         <v>59</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD13" t="s">
         <v>72</v>
@@ -1773,7 +1774,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="64" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1784,19 +1785,19 @@
         <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G14" t="s">
         <v>33</v>
       </c>
-      <c r="H14" t="s">
-        <v>102</v>
+      <c r="H14" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I14" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L14" t="s">
         <v>75</v>
@@ -1826,16 +1827,16 @@
         <v>59</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y14" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD14" t="s">
         <v>75</v>
@@ -1844,7 +1845,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>32</v>
       </c>
@@ -1855,19 +1856,19 @@
         <v>97</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
         <v>33</v>
       </c>
-      <c r="H15" t="s">
-        <v>102</v>
+      <c r="H15" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I15" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L15" t="s">
         <v>78</v>
@@ -1897,16 +1898,16 @@
         <v>59</v>
       </c>
       <c r="X15" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y15" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD15" t="s">
         <v>78</v>
@@ -1915,7 +1916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="135" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="112" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1926,19 +1927,19 @@
         <v>97</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
         <v>33</v>
       </c>
-      <c r="H16" t="s">
-        <v>102</v>
+      <c r="H16" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I16" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L16" t="s">
         <v>81</v>
@@ -1968,7 +1969,7 @@
         <v>84</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="Y16" s="3" t="s">
         <v>85</v>
@@ -1977,7 +1978,7 @@
         <v>86</v>
       </c>
       <c r="AA16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AD16" t="s">
         <v>81</v>
@@ -1986,7 +1987,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:31" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -1997,19 +1998,19 @@
         <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G17" t="s">
         <v>33</v>
       </c>
-      <c r="H17" t="s">
-        <v>102</v>
+      <c r="H17" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I17" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L17" t="s">
         <v>88</v>
@@ -2042,7 +2043,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="2:31" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31" ht="112" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -2053,19 +2054,19 @@
         <v>97</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
         <v>33</v>
       </c>
-      <c r="H18" t="s">
-        <v>102</v>
+      <c r="H18" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="I18" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="L18" t="s">
         <v>91</v>
@@ -2095,7 +2096,7 @@
         <v>94</v>
       </c>
       <c r="X18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="Y18" s="3" t="s">
         <v>95</v>
@@ -2104,7 +2105,7 @@
         <v>96</v>
       </c>
       <c r="AA18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD18" t="s">
         <v>91</v>
@@ -2113,7 +2114,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -2124,19 +2125,19 @@
         <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G19" t="s">
         <v>33</v>
       </c>
       <c r="H19" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I19" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L19" t="s">
         <v>34</v>
@@ -2148,7 +2149,7 @@
         <v>35</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Q19">
         <v>1</v>
@@ -2169,7 +2170,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -2180,19 +2181,19 @@
         <v>97</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
         <v>33</v>
       </c>
       <c r="H20" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I20" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L20" t="s">
         <v>49</v>
@@ -2201,10 +2202,10 @@
         <v>49</v>
       </c>
       <c r="N20" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Q20">
         <v>2</v>
@@ -2225,7 +2226,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -2236,19 +2237,19 @@
         <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G21" t="s">
         <v>33</v>
       </c>
       <c r="H21" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I21" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L21" t="s">
         <v>52</v>
@@ -2257,10 +2258,10 @@
         <v>52</v>
       </c>
       <c r="N21" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="Q21">
         <v>3</v>
@@ -2278,10 +2279,10 @@
         <v>48</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD21" t="s">
         <v>52</v>
@@ -2290,7 +2291,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -2301,19 +2302,19 @@
         <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
       </c>
       <c r="H22" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I22" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L22" t="s">
         <v>54</v>
@@ -2322,10 +2323,10 @@
         <v>54</v>
       </c>
       <c r="N22" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="Q22">
         <v>4</v>
@@ -2346,7 +2347,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>32</v>
       </c>
@@ -2357,19 +2358,19 @@
         <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G23" t="s">
         <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I23" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L23" t="s">
         <v>39</v>
@@ -2381,7 +2382,7 @@
         <v>40</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="Q23">
         <v>5</v>
@@ -2408,7 +2409,7 @@
         <v>45</v>
       </c>
       <c r="AA23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD23" t="s">
         <v>39</v>
@@ -2417,7 +2418,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>32</v>
       </c>
@@ -2428,19 +2429,19 @@
         <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
       </c>
       <c r="H24" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I24" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L24" t="s">
         <v>56</v>
@@ -2452,7 +2453,7 @@
         <v>57</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="Q24">
         <v>6</v>
@@ -2470,16 +2471,16 @@
         <v>59</v>
       </c>
       <c r="X24" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y24" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD24" t="s">
         <v>56</v>
@@ -2488,7 +2489,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>32</v>
       </c>
@@ -2499,19 +2500,19 @@
         <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
         <v>33</v>
       </c>
       <c r="H25" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I25" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L25" t="s">
         <v>60</v>
@@ -2523,7 +2524,7 @@
         <v>61</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="Q25">
         <v>7</v>
@@ -2541,16 +2542,16 @@
         <v>59</v>
       </c>
       <c r="X25" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y25" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD25" t="s">
         <v>60</v>
@@ -2559,7 +2560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -2570,19 +2571,19 @@
         <v>97</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G26" t="s">
         <v>33</v>
       </c>
       <c r="H26" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I26" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L26" t="s">
         <v>63</v>
@@ -2594,7 +2595,7 @@
         <v>64</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="Q26">
         <v>8</v>
@@ -2612,16 +2613,16 @@
         <v>59</v>
       </c>
       <c r="X26" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y26" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD26" t="s">
         <v>63</v>
@@ -2630,7 +2631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>32</v>
       </c>
@@ -2641,19 +2642,19 @@
         <v>97</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G27" t="s">
         <v>33</v>
       </c>
       <c r="H27" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I27" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L27" t="s">
         <v>66</v>
@@ -2665,7 +2666,7 @@
         <v>67</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q27">
         <v>9</v>
@@ -2683,16 +2684,16 @@
         <v>59</v>
       </c>
       <c r="X27" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y27" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD27" t="s">
         <v>66</v>
@@ -2701,7 +2702,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>32</v>
       </c>
@@ -2712,19 +2713,19 @@
         <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G28" t="s">
         <v>33</v>
       </c>
       <c r="H28" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I28" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L28" t="s">
         <v>69</v>
@@ -2736,7 +2737,7 @@
         <v>70</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Q28">
         <v>10</v>
@@ -2754,16 +2755,16 @@
         <v>59</v>
       </c>
       <c r="X28" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y28" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD28" t="s">
         <v>69</v>
@@ -2772,7 +2773,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>32</v>
       </c>
@@ -2783,19 +2784,19 @@
         <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G29" t="s">
         <v>33</v>
       </c>
       <c r="H29" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I29" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L29" t="s">
         <v>72</v>
@@ -2807,7 +2808,7 @@
         <v>73</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="Q29">
         <v>11</v>
@@ -2825,16 +2826,16 @@
         <v>59</v>
       </c>
       <c r="X29" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y29" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD29" t="s">
         <v>72</v>
@@ -2843,7 +2844,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -2854,19 +2855,19 @@
         <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G30" t="s">
         <v>33</v>
       </c>
       <c r="H30" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I30" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L30" t="s">
         <v>75</v>
@@ -2878,7 +2879,7 @@
         <v>76</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="Q30">
         <v>12</v>
@@ -2896,16 +2897,16 @@
         <v>59</v>
       </c>
       <c r="X30" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y30" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD30" t="s">
         <v>75</v>
@@ -2914,7 +2915,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>32</v>
       </c>
@@ -2924,17 +2925,20 @@
       <c r="D31" t="s">
         <v>97</v>
       </c>
+      <c r="E31" t="s">
+        <v>101</v>
+      </c>
       <c r="G31" t="s">
         <v>33</v>
       </c>
       <c r="H31" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I31" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L31" t="s">
         <v>78</v>
@@ -2946,7 +2950,7 @@
         <v>79</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="Q31">
         <v>13</v>
@@ -2964,16 +2968,16 @@
         <v>59</v>
       </c>
       <c r="X31" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Y31" s="3" t="s">
         <v>48</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD31" t="s">
         <v>78</v>
@@ -2982,7 +2986,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="2:31" ht="135" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31" ht="112" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -2993,19 +2997,19 @@
         <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G32" t="s">
         <v>33</v>
       </c>
       <c r="H32" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I32" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L32" t="s">
         <v>81</v>
@@ -3035,7 +3039,7 @@
         <v>84</v>
       </c>
       <c r="X32" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="Y32" s="3" t="s">
         <v>85</v>
@@ -3044,7 +3048,7 @@
         <v>86</v>
       </c>
       <c r="AA32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AD32" t="s">
         <v>81</v>
@@ -3053,7 +3057,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -3063,17 +3067,20 @@
       <c r="D33" t="s">
         <v>97</v>
       </c>
+      <c r="E33" t="s">
+        <v>101</v>
+      </c>
       <c r="G33" t="s">
         <v>33</v>
       </c>
       <c r="H33" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I33" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L33" t="s">
         <v>88</v>
@@ -3085,7 +3092,7 @@
         <v>89</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="Q33">
         <v>15</v>
@@ -3106,7 +3113,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="2:31" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:31" ht="112" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -3117,19 +3124,19 @@
         <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G34" t="s">
         <v>33</v>
       </c>
       <c r="H34" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="I34" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="L34" t="s">
         <v>91</v>
@@ -3141,7 +3148,7 @@
         <v>92</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="Q34">
         <v>16</v>
@@ -3159,7 +3166,7 @@
         <v>94</v>
       </c>
       <c r="X34" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="Y34" s="3" t="s">
         <v>95</v>
@@ -3168,7 +3175,7 @@
         <v>96</v>
       </c>
       <c r="AA34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD34" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
AE updated to include categories
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_AE.xlsx
+++ b/curation/draft/collection/collection_specialization_AE.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353760AE-C760-7D46-B5D1-4C63A954E0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05467C17-C6DF-A94D-A78E-FE1DF57D417C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="6640" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="5080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_AE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_AE!$A$1:$AG$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_AE!$A$1:$AH$34</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="136">
   <si>
     <t>package_date</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>Adverse Event Free Text Format (Normalized)</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -541,7 +544,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,12 +846,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AS1" sqref="AS1"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -861,27 +863,27 @@
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="23.83203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="27" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.6640625" customWidth="1"/>
-    <col min="18" max="18" width="17.33203125" customWidth="1"/>
-    <col min="20" max="20" width="12.5" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" customWidth="1"/>
-    <col min="24" max="24" width="30.83203125" customWidth="1"/>
-    <col min="25" max="25" width="21.33203125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="22.6640625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="19.5" customWidth="1"/>
-    <col min="28" max="28" width="20.83203125" customWidth="1"/>
-    <col min="29" max="29" width="14.6640625" customWidth="1"/>
-    <col min="30" max="30" width="18.83203125" customWidth="1"/>
-    <col min="31" max="31" width="16.83203125" customWidth="1"/>
-    <col min="32" max="32" width="15.5" customWidth="1"/>
-    <col min="33" max="33" width="11.6640625" customWidth="1"/>
+    <col min="10" max="11" width="18.1640625" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="23.83203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="27" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" customWidth="1"/>
+    <col min="21" max="21" width="12.5" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" customWidth="1"/>
+    <col min="25" max="25" width="30.83203125" customWidth="1"/>
+    <col min="26" max="26" width="21.33203125" style="3" customWidth="1"/>
+    <col min="27" max="27" width="22.6640625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="19.5" customWidth="1"/>
+    <col min="29" max="29" width="20.83203125" customWidth="1"/>
+    <col min="30" max="30" width="14.6640625" customWidth="1"/>
+    <col min="31" max="31" width="18.83203125" customWidth="1"/>
+    <col min="32" max="32" width="16.83203125" customWidth="1"/>
+    <col min="33" max="33" width="15.5" customWidth="1"/>
+    <col min="34" max="34" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,77 +914,80 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>121</v>
       </c>
@@ -998,53 +1003,53 @@
       <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="L2" t="s">
-        <v>46</v>
       </c>
       <c r="M2" t="s">
         <v>46</v>
       </c>
       <c r="N2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
         <v>121</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>42</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>38</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>59</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>98</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -1066,41 +1071,41 @@
       <c r="I3" t="s">
         <v>130</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L3" t="s">
-        <v>34</v>
       </c>
       <c r="M3" t="s">
         <v>34</v>
       </c>
       <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>1</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>37</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>38</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>200</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>34</v>
       </c>
       <c r="AE3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -1116,47 +1121,47 @@
       <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" t="s">
         <v>129</v>
       </c>
       <c r="I4" t="s">
         <v>130</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L4" t="s">
-        <v>49</v>
       </c>
       <c r="M4" t="s">
         <v>49</v>
       </c>
       <c r="N4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" t="s">
         <v>118</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>37</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>51</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>10</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>49</v>
       </c>
       <c r="AE4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" ht="48" x14ac:dyDescent="0.2">
+      <c r="AF4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -1172,56 +1177,56 @@
       <c r="G5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" t="s">
         <v>129</v>
       </c>
       <c r="I5" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L5" t="s">
-        <v>52</v>
       </c>
       <c r="M5" t="s">
         <v>52</v>
       </c>
       <c r="N5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" t="s">
         <v>119</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>3</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>42</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>38</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>1</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Z5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AA5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>98</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>127</v>
       </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -1237,47 +1242,47 @@
       <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" t="s">
         <v>129</v>
       </c>
       <c r="I6" t="s">
         <v>130</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L6" t="s">
-        <v>54</v>
       </c>
       <c r="M6" t="s">
         <v>54</v>
       </c>
       <c r="N6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" t="s">
         <v>120</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>4</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>37</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>51</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>10</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>54</v>
       </c>
       <c r="AE6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -1293,62 +1298,62 @@
       <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" t="s">
         <v>129</v>
       </c>
       <c r="I7" t="s">
         <v>130</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L7" t="s">
-        <v>39</v>
       </c>
       <c r="M7" t="s">
         <v>39</v>
       </c>
       <c r="N7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>5</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>42</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>38</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>200</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>43</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>39</v>
       </c>
-      <c r="Y7" s="3" t="s">
+      <c r="Z7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Z7" s="3" t="s">
+      <c r="AA7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>98</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>39</v>
       </c>
       <c r="AE7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -1364,62 +1369,62 @@
       <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" t="s">
         <v>129</v>
       </c>
       <c r="I8" t="s">
         <v>130</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L8" t="s">
-        <v>56</v>
       </c>
       <c r="M8" t="s">
         <v>56</v>
       </c>
       <c r="N8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" t="s">
         <v>57</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>6</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>37</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>38</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>1</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>59</v>
       </c>
-      <c r="X8" s="4" t="s">
+      <c r="Y8" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y8" s="3" t="s">
+      <c r="Z8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z8" s="3" t="s">
+      <c r="AA8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>98</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>56</v>
       </c>
       <c r="AE8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>32</v>
       </c>
@@ -1435,62 +1440,62 @@
       <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" t="s">
         <v>129</v>
       </c>
       <c r="I9" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L9" t="s">
-        <v>60</v>
       </c>
       <c r="M9" t="s">
         <v>60</v>
       </c>
       <c r="N9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" t="s">
         <v>61</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>7</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>42</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>38</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>1</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>59</v>
       </c>
-      <c r="X9" s="4" t="s">
+      <c r="Y9" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y9" s="3" t="s">
+      <c r="Z9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z9" s="3" t="s">
+      <c r="AA9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>98</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>60</v>
       </c>
       <c r="AE9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -1506,62 +1511,62 @@
       <c r="G10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" t="s">
         <v>129</v>
       </c>
       <c r="I10" t="s">
         <v>130</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L10" t="s">
-        <v>63</v>
       </c>
       <c r="M10" t="s">
         <v>63</v>
       </c>
       <c r="N10" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" t="s">
         <v>64</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>8</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>42</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>38</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>1</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>59</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="Y10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y10" s="3" t="s">
+      <c r="Z10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AA10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>98</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>63</v>
       </c>
       <c r="AE10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" ht="64" x14ac:dyDescent="0.2">
+      <c r="AF10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -1577,62 +1582,62 @@
       <c r="G11" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" t="s">
         <v>129</v>
       </c>
       <c r="I11" t="s">
         <v>130</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L11" t="s">
-        <v>66</v>
       </c>
       <c r="M11" t="s">
         <v>66</v>
       </c>
       <c r="N11" t="s">
+        <v>66</v>
+      </c>
+      <c r="O11" t="s">
         <v>67</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>9</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>42</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>38</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>1</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>59</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="Y11" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y11" s="3" t="s">
+      <c r="Z11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z11" s="3" t="s">
+      <c r="AA11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>98</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>66</v>
       </c>
       <c r="AE11" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" ht="48" x14ac:dyDescent="0.2">
+      <c r="AF11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1648,62 +1653,62 @@
       <c r="G12" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" t="s">
         <v>129</v>
       </c>
       <c r="I12" t="s">
         <v>130</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L12" t="s">
-        <v>69</v>
       </c>
       <c r="M12" t="s">
         <v>69</v>
       </c>
       <c r="N12" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" t="s">
         <v>70</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>10</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>42</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>38</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>1</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>59</v>
       </c>
-      <c r="X12" s="4" t="s">
+      <c r="Y12" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y12" s="3" t="s">
+      <c r="Z12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z12" s="3" t="s">
+      <c r="AA12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>98</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>69</v>
       </c>
       <c r="AE12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" ht="48" x14ac:dyDescent="0.2">
+      <c r="AF12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -1719,62 +1724,62 @@
       <c r="G13" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" t="s">
         <v>129</v>
       </c>
       <c r="I13" t="s">
         <v>130</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L13" t="s">
-        <v>72</v>
       </c>
       <c r="M13" t="s">
         <v>72</v>
       </c>
       <c r="N13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O13" t="s">
         <v>73</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="P13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>11</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>42</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>38</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>1</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>59</v>
       </c>
-      <c r="X13" s="4" t="s">
+      <c r="Y13" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y13" s="3" t="s">
+      <c r="Z13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z13" s="3" t="s">
+      <c r="AA13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AB13" t="s">
         <v>98</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>72</v>
       </c>
       <c r="AE13" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" ht="64" x14ac:dyDescent="0.2">
+      <c r="AF13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="64" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1790,62 +1795,62 @@
       <c r="G14" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" t="s">
         <v>129</v>
       </c>
       <c r="I14" t="s">
         <v>130</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L14" t="s">
-        <v>75</v>
       </c>
       <c r="M14" t="s">
         <v>75</v>
       </c>
       <c r="N14" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" t="s">
         <v>76</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="P14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>12</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>42</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>38</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>1</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>59</v>
       </c>
-      <c r="X14" s="4" t="s">
+      <c r="Y14" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y14" s="3" t="s">
+      <c r="Z14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z14" s="3" t="s">
+      <c r="AA14" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AB14" t="s">
         <v>98</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>75</v>
       </c>
       <c r="AE14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>32</v>
       </c>
@@ -1861,62 +1866,62 @@
       <c r="G15" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" t="s">
         <v>129</v>
       </c>
       <c r="I15" t="s">
         <v>130</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L15" t="s">
-        <v>78</v>
       </c>
       <c r="M15" t="s">
         <v>78</v>
       </c>
       <c r="N15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" t="s">
         <v>79</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>13</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>37</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>38</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>1</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>59</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="Y15" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y15" s="3" t="s">
+      <c r="Z15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z15" s="3" t="s">
+      <c r="AA15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>98</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>78</v>
       </c>
       <c r="AE15" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" ht="112" x14ac:dyDescent="0.2">
+      <c r="AF15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="112" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1932,62 +1937,62 @@
       <c r="G16" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" t="s">
         <v>129</v>
       </c>
       <c r="I16" t="s">
         <v>130</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L16" t="s">
-        <v>81</v>
       </c>
       <c r="M16" t="s">
         <v>81</v>
       </c>
       <c r="N16" t="s">
+        <v>81</v>
+      </c>
+      <c r="O16" t="s">
         <v>82</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="P16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>14</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>37</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>38</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>200</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>84</v>
       </c>
-      <c r="X16" s="4" t="s">
+      <c r="Y16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="Y16" s="3" t="s">
+      <c r="Z16" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Z16" s="3" t="s">
+      <c r="AA16" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
         <v>99</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>81</v>
       </c>
       <c r="AE16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="2:31" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -2003,47 +2008,47 @@
       <c r="G17" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" t="s">
         <v>129</v>
       </c>
       <c r="I17" t="s">
         <v>130</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L17" t="s">
-        <v>88</v>
       </c>
       <c r="M17" t="s">
         <v>88</v>
       </c>
       <c r="N17" t="s">
+        <v>88</v>
+      </c>
+      <c r="O17" t="s">
         <v>89</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="P17" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>15</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>42</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>38</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>200</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>88</v>
       </c>
       <c r="AE17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="2:31" ht="112" x14ac:dyDescent="0.2">
+      <c r="AF17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" ht="112" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -2059,62 +2064,62 @@
       <c r="G18" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" t="s">
         <v>129</v>
       </c>
       <c r="I18" t="s">
         <v>130</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="L18" t="s">
-        <v>91</v>
       </c>
       <c r="M18" t="s">
         <v>91</v>
       </c>
       <c r="N18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O18" t="s">
         <v>92</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="P18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>16</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>42</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>38</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>200</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>94</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>124</v>
       </c>
-      <c r="Y18" s="3" t="s">
+      <c r="Z18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Z18" s="3" t="s">
+      <c r="AA18" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>98</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>91</v>
       </c>
       <c r="AE18" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -2136,41 +2141,41 @@
       <c r="I19" t="s">
         <v>133</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L19" t="s">
-        <v>34</v>
       </c>
       <c r="M19" t="s">
         <v>34</v>
       </c>
       <c r="N19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="Q19" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>1</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>37</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>38</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>200</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>34</v>
       </c>
       <c r="AE19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -2192,41 +2197,41 @@
       <c r="I20" t="s">
         <v>133</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L20" t="s">
-        <v>49</v>
       </c>
       <c r="M20" t="s">
         <v>49</v>
       </c>
       <c r="N20" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" t="s">
         <v>118</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="Q20" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>2</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>37</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>51</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>10</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>49</v>
       </c>
       <c r="AE20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -2248,50 +2253,50 @@
       <c r="I21" t="s">
         <v>133</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L21" t="s">
-        <v>52</v>
       </c>
       <c r="M21" t="s">
         <v>52</v>
       </c>
       <c r="N21" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21" t="s">
         <v>119</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="Q21" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>3</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>42</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>38</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>1</v>
       </c>
-      <c r="Y21" s="3" t="s">
+      <c r="Z21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z21" s="3" t="s">
+      <c r="AA21" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AB21" t="s">
         <v>98</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>52</v>
       </c>
       <c r="AE21" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -2313,41 +2318,41 @@
       <c r="I22" t="s">
         <v>133</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L22" t="s">
-        <v>54</v>
       </c>
       <c r="M22" t="s">
         <v>54</v>
       </c>
       <c r="N22" t="s">
+        <v>54</v>
+      </c>
+      <c r="O22" t="s">
         <v>120</v>
       </c>
-      <c r="P22" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>4</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>37</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>51</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>10</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>54</v>
       </c>
       <c r="AE22" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>32</v>
       </c>
@@ -2369,56 +2374,56 @@
       <c r="I23" t="s">
         <v>133</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L23" t="s">
-        <v>39</v>
       </c>
       <c r="M23" t="s">
         <v>39</v>
       </c>
       <c r="N23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" t="s">
         <v>40</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="Q23" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>5</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>42</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>38</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>200</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>43</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>39</v>
       </c>
-      <c r="Y23" s="3" t="s">
+      <c r="Z23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Z23" s="3" t="s">
+      <c r="AA23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AB23" t="s">
         <v>98</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>39</v>
       </c>
       <c r="AE23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>32</v>
       </c>
@@ -2440,56 +2445,56 @@
       <c r="I24" t="s">
         <v>133</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L24" t="s">
-        <v>56</v>
       </c>
       <c r="M24" t="s">
         <v>56</v>
       </c>
       <c r="N24" t="s">
+        <v>56</v>
+      </c>
+      <c r="O24" t="s">
         <v>57</v>
       </c>
-      <c r="P24" s="3" t="s">
+      <c r="Q24" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>6</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>37</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>38</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>1</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>59</v>
       </c>
-      <c r="X24" s="4" t="s">
+      <c r="Y24" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y24" s="3" t="s">
+      <c r="Z24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z24" s="3" t="s">
+      <c r="AA24" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>98</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>56</v>
       </c>
       <c r="AE24" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>32</v>
       </c>
@@ -2511,56 +2516,56 @@
       <c r="I25" t="s">
         <v>133</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L25" t="s">
-        <v>60</v>
       </c>
       <c r="M25" t="s">
         <v>60</v>
       </c>
       <c r="N25" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" t="s">
         <v>61</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="Q25" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>7</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>42</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>38</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>1</v>
       </c>
-      <c r="W25" t="s">
+      <c r="X25" t="s">
         <v>59</v>
       </c>
-      <c r="X25" s="4" t="s">
+      <c r="Y25" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y25" s="3" t="s">
+      <c r="Z25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z25" s="3" t="s">
+      <c r="AA25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AB25" t="s">
         <v>98</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>60</v>
       </c>
       <c r="AE25" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -2582,56 +2587,56 @@
       <c r="I26" t="s">
         <v>133</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L26" t="s">
-        <v>63</v>
       </c>
       <c r="M26" t="s">
         <v>63</v>
       </c>
       <c r="N26" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" t="s">
         <v>64</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>8</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>42</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>38</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>1</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>59</v>
       </c>
-      <c r="X26" s="4" t="s">
+      <c r="Y26" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y26" s="3" t="s">
+      <c r="Z26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z26" s="3" t="s">
+      <c r="AA26" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="AB26" t="s">
         <v>98</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>63</v>
       </c>
       <c r="AE26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>32</v>
       </c>
@@ -2653,56 +2658,56 @@
       <c r="I27" t="s">
         <v>133</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="L27" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L27" t="s">
-        <v>66</v>
       </c>
       <c r="M27" t="s">
         <v>66</v>
       </c>
       <c r="N27" t="s">
+        <v>66</v>
+      </c>
+      <c r="O27" t="s">
         <v>67</v>
       </c>
-      <c r="P27" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>9</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>42</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>38</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>1</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>59</v>
       </c>
-      <c r="X27" s="4" t="s">
+      <c r="Y27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y27" s="3" t="s">
+      <c r="Z27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z27" s="3" t="s">
+      <c r="AA27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>98</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>66</v>
       </c>
       <c r="AE27" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>32</v>
       </c>
@@ -2724,56 +2729,56 @@
       <c r="I28" t="s">
         <v>133</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="L28" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L28" t="s">
-        <v>69</v>
       </c>
       <c r="M28" t="s">
         <v>69</v>
       </c>
       <c r="N28" t="s">
+        <v>69</v>
+      </c>
+      <c r="O28" t="s">
         <v>70</v>
       </c>
-      <c r="P28" s="3" t="s">
+      <c r="Q28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>10</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>42</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>38</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>1</v>
       </c>
-      <c r="W28" t="s">
+      <c r="X28" t="s">
         <v>59</v>
       </c>
-      <c r="X28" s="4" t="s">
+      <c r="Y28" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y28" s="3" t="s">
+      <c r="Z28" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z28" s="3" t="s">
+      <c r="AA28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AB28" t="s">
         <v>98</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>69</v>
       </c>
       <c r="AE28" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>32</v>
       </c>
@@ -2795,56 +2800,56 @@
       <c r="I29" t="s">
         <v>133</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="L29" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L29" t="s">
-        <v>72</v>
       </c>
       <c r="M29" t="s">
         <v>72</v>
       </c>
       <c r="N29" t="s">
+        <v>72</v>
+      </c>
+      <c r="O29" t="s">
         <v>73</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="Q29" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>11</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>42</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>38</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>1</v>
       </c>
-      <c r="W29" t="s">
+      <c r="X29" t="s">
         <v>59</v>
       </c>
-      <c r="X29" s="4" t="s">
+      <c r="Y29" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y29" s="3" t="s">
+      <c r="Z29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z29" s="3" t="s">
+      <c r="AA29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AB29" t="s">
         <v>98</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>72</v>
       </c>
       <c r="AE29" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -2866,56 +2871,56 @@
       <c r="I30" t="s">
         <v>133</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="L30" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L30" t="s">
-        <v>75</v>
       </c>
       <c r="M30" t="s">
         <v>75</v>
       </c>
       <c r="N30" t="s">
+        <v>75</v>
+      </c>
+      <c r="O30" t="s">
         <v>76</v>
       </c>
-      <c r="P30" s="3" t="s">
+      <c r="Q30" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>12</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>42</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>38</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>1</v>
       </c>
-      <c r="W30" t="s">
+      <c r="X30" t="s">
         <v>59</v>
       </c>
-      <c r="X30" s="4" t="s">
+      <c r="Y30" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y30" s="3" t="s">
+      <c r="Z30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z30" s="3" t="s">
+      <c r="AA30" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AB30" t="s">
         <v>98</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>75</v>
       </c>
       <c r="AE30" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>32</v>
       </c>
@@ -2937,56 +2942,56 @@
       <c r="I31" t="s">
         <v>133</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="L31" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L31" t="s">
-        <v>78</v>
       </c>
       <c r="M31" t="s">
         <v>78</v>
       </c>
       <c r="N31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O31" t="s">
         <v>79</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="Q31" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>13</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>37</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>38</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>1</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>59</v>
       </c>
-      <c r="X31" s="4" t="s">
+      <c r="Y31" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Y31" s="3" t="s">
+      <c r="Z31" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z31" s="3" t="s">
+      <c r="AA31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AB31" t="s">
         <v>98</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>78</v>
       </c>
       <c r="AE31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="2:31" ht="112" x14ac:dyDescent="0.2">
+      <c r="AF31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" ht="112" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -3008,56 +3013,56 @@
       <c r="I32" t="s">
         <v>133</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="L32" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L32" t="s">
-        <v>81</v>
       </c>
       <c r="M32" t="s">
         <v>81</v>
       </c>
       <c r="N32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O32" t="s">
         <v>82</v>
       </c>
-      <c r="P32" s="3" t="s">
+      <c r="Q32" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>14</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>37</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>38</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>200</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>84</v>
       </c>
-      <c r="X32" s="4" t="s">
+      <c r="Y32" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="Y32" s="3" t="s">
+      <c r="Z32" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Z32" s="3" t="s">
+      <c r="AA32" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AB32" t="s">
         <v>99</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>81</v>
       </c>
       <c r="AE32" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="2:31" ht="32" x14ac:dyDescent="0.2">
+      <c r="AF32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -3079,41 +3084,41 @@
       <c r="I33" t="s">
         <v>133</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L33" t="s">
-        <v>88</v>
       </c>
       <c r="M33" t="s">
         <v>88</v>
       </c>
       <c r="N33" t="s">
+        <v>88</v>
+      </c>
+      <c r="O33" t="s">
         <v>89</v>
       </c>
-      <c r="P33" s="3" t="s">
+      <c r="Q33" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <v>15</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>42</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>38</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>200</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>88</v>
       </c>
       <c r="AE33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="2:31" ht="112" x14ac:dyDescent="0.2">
+      <c r="AF33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:32" ht="112" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -3135,57 +3140,57 @@
       <c r="I34" t="s">
         <v>133</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="L34" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="L34" t="s">
-        <v>91</v>
       </c>
       <c r="M34" t="s">
         <v>91</v>
       </c>
       <c r="N34" t="s">
+        <v>91</v>
+      </c>
+      <c r="O34" t="s">
         <v>92</v>
       </c>
-      <c r="P34" s="3" t="s">
+      <c r="Q34" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>16</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>42</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>38</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>200</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>94</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>124</v>
       </c>
-      <c r="Y34" s="3" t="s">
+      <c r="Z34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Z34" s="3" t="s">
+      <c r="AA34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AB34" t="s">
         <v>98</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>91</v>
       </c>
       <c r="AE34" t="s">
         <v>91</v>
       </c>
+      <c r="AF34" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AH34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added derivation columns (blank)
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_AE.xlsx
+++ b/curation/draft/collection/collection_specialization_AE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05467C17-C6DF-A94D-A78E-FE1DF57D417C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA93A3A-20F4-BF4F-BB74-4AE7ABEF4786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="5080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Collection_AE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_AE!$A$1:$AH$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_AE!$A$1:$AJ$34</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="138">
   <si>
     <t>package_date</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -846,12 +852,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH34"/>
+  <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AS1" sqref="AS1"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomLeft" activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -870,20 +876,21 @@
     <col min="18" max="18" width="16.6640625" customWidth="1"/>
     <col min="19" max="19" width="17.33203125" customWidth="1"/>
     <col min="21" max="21" width="12.5" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" customWidth="1"/>
-    <col min="25" max="25" width="30.83203125" customWidth="1"/>
-    <col min="26" max="26" width="21.33203125" style="3" customWidth="1"/>
-    <col min="27" max="27" width="22.6640625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="19.5" customWidth="1"/>
-    <col min="29" max="29" width="20.83203125" customWidth="1"/>
-    <col min="30" max="30" width="14.6640625" customWidth="1"/>
-    <col min="31" max="31" width="18.83203125" customWidth="1"/>
-    <col min="32" max="32" width="16.83203125" customWidth="1"/>
-    <col min="33" max="33" width="15.5" customWidth="1"/>
-    <col min="34" max="34" width="11.6640625" customWidth="1"/>
+    <col min="23" max="24" width="16.6640625" customWidth="1"/>
+    <col min="25" max="25" width="22.83203125" customWidth="1"/>
+    <col min="27" max="27" width="30.83203125" customWidth="1"/>
+    <col min="28" max="28" width="21.33203125" style="3" customWidth="1"/>
+    <col min="29" max="29" width="22.6640625" style="3" customWidth="1"/>
+    <col min="30" max="30" width="19.5" customWidth="1"/>
+    <col min="31" max="31" width="20.83203125" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
+    <col min="33" max="33" width="18.83203125" customWidth="1"/>
+    <col min="34" max="34" width="16.83203125" customWidth="1"/>
+    <col min="35" max="35" width="15.5" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,40 +961,46 @@
         <v>20</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>121</v>
       </c>
@@ -1030,26 +1043,26 @@
       <c r="U2">
         <v>1</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>98</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -1098,14 +1111,14 @@
       <c r="U3">
         <v>200</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>34</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -1154,14 +1167,14 @@
       <c r="U4">
         <v>10</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>49</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -1210,23 +1223,23 @@
       <c r="U5">
         <v>1</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AD5" t="s">
         <v>98</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>127</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AH5" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -1275,14 +1288,14 @@
       <c r="U6">
         <v>10</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>54</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -1331,29 +1344,29 @@
       <c r="U7">
         <v>200</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>43</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA7" t="s">
         <v>39</v>
       </c>
-      <c r="Z7" s="3" t="s">
+      <c r="AB7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AA7" s="3" t="s">
+      <c r="AC7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AD7" t="s">
         <v>98</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>39</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -1402,29 +1415,29 @@
       <c r="U8">
         <v>1</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>59</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="AA8" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z8" s="3" t="s">
+      <c r="AB8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA8" s="3" t="s">
+      <c r="AC8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AD8" t="s">
         <v>98</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>56</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>32</v>
       </c>
@@ -1473,29 +1486,29 @@
       <c r="U9">
         <v>1</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Z9" t="s">
         <v>59</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="AA9" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z9" s="3" t="s">
+      <c r="AB9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA9" s="3" t="s">
+      <c r="AC9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AD9" t="s">
         <v>98</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AG9" t="s">
         <v>60</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AH9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -1544,29 +1557,29 @@
       <c r="U10">
         <v>1</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Z10" t="s">
         <v>59</v>
       </c>
-      <c r="Y10" s="4" t="s">
+      <c r="AA10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AB10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA10" s="3" t="s">
+      <c r="AC10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AD10" t="s">
         <v>98</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AG10" t="s">
         <v>63</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -1615,29 +1628,29 @@
       <c r="U11">
         <v>1</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z11" t="s">
         <v>59</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="AA11" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z11" s="3" t="s">
+      <c r="AB11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA11" s="3" t="s">
+      <c r="AC11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AD11" t="s">
         <v>98</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AG11" t="s">
         <v>66</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AH11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1686,29 +1699,29 @@
       <c r="U12">
         <v>1</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Z12" t="s">
         <v>59</v>
       </c>
-      <c r="Y12" s="4" t="s">
+      <c r="AA12" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z12" s="3" t="s">
+      <c r="AB12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA12" s="3" t="s">
+      <c r="AC12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AD12" t="s">
         <v>98</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>69</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AH12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -1757,29 +1770,29 @@
       <c r="U13">
         <v>1</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Z13" t="s">
         <v>59</v>
       </c>
-      <c r="Y13" s="4" t="s">
+      <c r="AA13" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z13" s="3" t="s">
+      <c r="AB13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA13" s="3" t="s">
+      <c r="AC13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AD13" t="s">
         <v>98</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AG13" t="s">
         <v>72</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AH13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="64" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1828,29 +1841,29 @@
       <c r="U14">
         <v>1</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Z14" t="s">
         <v>59</v>
       </c>
-      <c r="Y14" s="4" t="s">
+      <c r="AA14" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z14" s="3" t="s">
+      <c r="AB14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA14" s="3" t="s">
+      <c r="AC14" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AD14" t="s">
         <v>98</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AG14" t="s">
         <v>75</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AH14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>32</v>
       </c>
@@ -1899,29 +1912,29 @@
       <c r="U15">
         <v>1</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Z15" t="s">
         <v>59</v>
       </c>
-      <c r="Y15" s="4" t="s">
+      <c r="AA15" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z15" s="3" t="s">
+      <c r="AB15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA15" s="3" t="s">
+      <c r="AC15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AD15" t="s">
         <v>98</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AG15" t="s">
         <v>78</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AH15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="112" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1970,29 +1983,29 @@
       <c r="U16">
         <v>200</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Z16" t="s">
         <v>84</v>
       </c>
-      <c r="Y16" s="4" t="s">
+      <c r="AA16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="Z16" s="3" t="s">
+      <c r="AB16" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AA16" s="3" t="s">
+      <c r="AC16" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AD16" t="s">
         <v>99</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AG16" t="s">
         <v>81</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AH16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:32" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:34" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -2041,14 +2054,14 @@
       <c r="U17">
         <v>200</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AG17" t="s">
         <v>88</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AH17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="2:32" ht="112" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:34" ht="112" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -2097,29 +2110,29 @@
       <c r="U18">
         <v>200</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Z18" t="s">
         <v>94</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="AA18" t="s">
         <v>124</v>
       </c>
-      <c r="Z18" s="3" t="s">
+      <c r="AB18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AA18" s="3" t="s">
+      <c r="AC18" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AD18" t="s">
         <v>98</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AG18" t="s">
         <v>91</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AH18" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -2168,14 +2181,14 @@
       <c r="U19">
         <v>200</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AG19" t="s">
         <v>34</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AH19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -2224,14 +2237,14 @@
       <c r="U20">
         <v>10</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AG20" t="s">
         <v>49</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AH20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -2280,23 +2293,23 @@
       <c r="U21">
         <v>1</v>
       </c>
-      <c r="Z21" s="3" t="s">
+      <c r="AB21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA21" s="3" t="s">
+      <c r="AC21" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AD21" t="s">
         <v>98</v>
       </c>
-      <c r="AE21" t="s">
+      <c r="AG21" t="s">
         <v>52</v>
       </c>
-      <c r="AF21" t="s">
+      <c r="AH21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -2345,14 +2358,14 @@
       <c r="U22">
         <v>10</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AG22" t="s">
         <v>54</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AH22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>32</v>
       </c>
@@ -2401,29 +2414,29 @@
       <c r="U23">
         <v>200</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Z23" t="s">
         <v>43</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="AA23" t="s">
         <v>39</v>
       </c>
-      <c r="Z23" s="3" t="s">
+      <c r="AB23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AA23" s="3" t="s">
+      <c r="AC23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AD23" t="s">
         <v>98</v>
       </c>
-      <c r="AE23" t="s">
+      <c r="AG23" t="s">
         <v>39</v>
       </c>
-      <c r="AF23" t="s">
+      <c r="AH23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>32</v>
       </c>
@@ -2472,29 +2485,29 @@
       <c r="U24">
         <v>1</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Z24" t="s">
         <v>59</v>
       </c>
-      <c r="Y24" s="4" t="s">
+      <c r="AA24" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z24" s="3" t="s">
+      <c r="AB24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA24" s="3" t="s">
+      <c r="AC24" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AD24" t="s">
         <v>98</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AG24" t="s">
         <v>56</v>
       </c>
-      <c r="AF24" t="s">
+      <c r="AH24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>32</v>
       </c>
@@ -2543,29 +2556,29 @@
       <c r="U25">
         <v>1</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Z25" t="s">
         <v>59</v>
       </c>
-      <c r="Y25" s="4" t="s">
+      <c r="AA25" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z25" s="3" t="s">
+      <c r="AB25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA25" s="3" t="s">
+      <c r="AC25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="AD25" t="s">
         <v>98</v>
       </c>
-      <c r="AE25" t="s">
+      <c r="AG25" t="s">
         <v>60</v>
       </c>
-      <c r="AF25" t="s">
+      <c r="AH25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -2614,29 +2627,29 @@
       <c r="U26">
         <v>1</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Z26" t="s">
         <v>59</v>
       </c>
-      <c r="Y26" s="4" t="s">
+      <c r="AA26" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z26" s="3" t="s">
+      <c r="AB26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA26" s="3" t="s">
+      <c r="AC26" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB26" t="s">
+      <c r="AD26" t="s">
         <v>98</v>
       </c>
-      <c r="AE26" t="s">
+      <c r="AG26" t="s">
         <v>63</v>
       </c>
-      <c r="AF26" t="s">
+      <c r="AH26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>32</v>
       </c>
@@ -2685,29 +2698,29 @@
       <c r="U27">
         <v>1</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Z27" t="s">
         <v>59</v>
       </c>
-      <c r="Y27" s="4" t="s">
+      <c r="AA27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z27" s="3" t="s">
+      <c r="AB27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA27" s="3" t="s">
+      <c r="AC27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AD27" t="s">
         <v>98</v>
       </c>
-      <c r="AE27" t="s">
+      <c r="AG27" t="s">
         <v>66</v>
       </c>
-      <c r="AF27" t="s">
+      <c r="AH27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>32</v>
       </c>
@@ -2756,29 +2769,29 @@
       <c r="U28">
         <v>1</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Z28" t="s">
         <v>59</v>
       </c>
-      <c r="Y28" s="4" t="s">
+      <c r="AA28" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z28" s="3" t="s">
+      <c r="AB28" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA28" s="3" t="s">
+      <c r="AC28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB28" t="s">
+      <c r="AD28" t="s">
         <v>98</v>
       </c>
-      <c r="AE28" t="s">
+      <c r="AG28" t="s">
         <v>69</v>
       </c>
-      <c r="AF28" t="s">
+      <c r="AH28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>32</v>
       </c>
@@ -2827,29 +2840,29 @@
       <c r="U29">
         <v>1</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Z29" t="s">
         <v>59</v>
       </c>
-      <c r="Y29" s="4" t="s">
+      <c r="AA29" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z29" s="3" t="s">
+      <c r="AB29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA29" s="3" t="s">
+      <c r="AC29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB29" t="s">
+      <c r="AD29" t="s">
         <v>98</v>
       </c>
-      <c r="AE29" t="s">
+      <c r="AG29" t="s">
         <v>72</v>
       </c>
-      <c r="AF29" t="s">
+      <c r="AH29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -2898,29 +2911,29 @@
       <c r="U30">
         <v>1</v>
       </c>
-      <c r="X30" t="s">
+      <c r="Z30" t="s">
         <v>59</v>
       </c>
-      <c r="Y30" s="4" t="s">
+      <c r="AA30" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z30" s="3" t="s">
+      <c r="AB30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA30" s="3" t="s">
+      <c r="AC30" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB30" t="s">
+      <c r="AD30" t="s">
         <v>98</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AG30" t="s">
         <v>75</v>
       </c>
-      <c r="AF30" t="s">
+      <c r="AH30" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>32</v>
       </c>
@@ -2969,29 +2982,29 @@
       <c r="U31">
         <v>1</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Z31" t="s">
         <v>59</v>
       </c>
-      <c r="Y31" s="4" t="s">
+      <c r="AA31" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Z31" s="3" t="s">
+      <c r="AB31" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA31" s="3" t="s">
+      <c r="AC31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AD31" t="s">
         <v>98</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AG31" t="s">
         <v>78</v>
       </c>
-      <c r="AF31" t="s">
+      <c r="AH31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="2:32" ht="112" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:34" ht="112" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -3040,29 +3053,29 @@
       <c r="U32">
         <v>200</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Z32" t="s">
         <v>84</v>
       </c>
-      <c r="Y32" s="4" t="s">
+      <c r="AA32" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="Z32" s="3" t="s">
+      <c r="AB32" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AA32" s="3" t="s">
+      <c r="AC32" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AD32" t="s">
         <v>99</v>
       </c>
-      <c r="AE32" t="s">
+      <c r="AG32" t="s">
         <v>81</v>
       </c>
-      <c r="AF32" t="s">
+      <c r="AH32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -3111,14 +3124,14 @@
       <c r="U33">
         <v>200</v>
       </c>
-      <c r="AE33" t="s">
+      <c r="AG33" t="s">
         <v>88</v>
       </c>
-      <c r="AF33" t="s">
+      <c r="AH33" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="2:32" ht="112" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:34" ht="112" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -3167,30 +3180,30 @@
       <c r="U34">
         <v>200</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Z34" t="s">
         <v>94</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="AA34" t="s">
         <v>124</v>
       </c>
-      <c r="Z34" s="3" t="s">
+      <c r="AB34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AA34" s="3" t="s">
+      <c r="AC34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AD34" t="s">
         <v>98</v>
       </c>
-      <c r="AE34" t="s">
+      <c r="AG34" t="s">
         <v>91</v>
       </c>
-      <c r="AF34" t="s">
+      <c r="AH34" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated mapping for Ongoing
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_AE.xlsx
+++ b/curation/draft/collection/collection_specialization_AE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA93A3A-20F4-BF4F-BB74-4AE7ABEF4786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CC71D4-14C4-8E48-B06E-6935203BCF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="5080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,12 +419,6 @@
     <t>Adverse Event Yes No Indicator</t>
   </si>
   <si>
-    <t>AEENRTPT; AEENRF</t>
-  </si>
-  <si>
-    <t>[NOT SUBMITTED];AEENRTPT; AEENRF</t>
-  </si>
-  <si>
     <t>AE_DENORMALIZED</t>
   </si>
   <si>
@@ -450,6 +444,12 @@
   </si>
   <si>
     <t>derivation_description</t>
+  </si>
+  <si>
+    <t>AEENRTPT; AEENRF;AEENTPT</t>
+  </si>
+  <si>
+    <t>[NOT SUBMITTED];AEENRTPT; AEENRF;AEENTPT</t>
   </si>
 </sst>
 </file>
@@ -854,10 +854,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AS1" sqref="AS1"/>
-      <selection pane="bottomLeft" activeCell="X24" sqref="X24"/>
+      <selection pane="bottomLeft" activeCell="AF35" sqref="AF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -922,7 +922,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
@@ -961,10 +961,10 @@
         <v>20</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>21</v>
@@ -1079,13 +1079,13 @@
         <v>33</v>
       </c>
       <c r="H3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I3" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M3" t="s">
         <v>34</v>
@@ -1135,13 +1135,13 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I4" t="s">
-        <v>130</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M4" t="s">
         <v>49</v>
@@ -1191,13 +1191,13 @@
         <v>33</v>
       </c>
       <c r="H5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I5" t="s">
-        <v>130</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M5" t="s">
         <v>52</v>
@@ -1233,10 +1233,10 @@
         <v>98</v>
       </c>
       <c r="AG5" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="32" x14ac:dyDescent="0.2">
@@ -1256,13 +1256,13 @@
         <v>33</v>
       </c>
       <c r="H6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I6" t="s">
-        <v>130</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M6" t="s">
         <v>54</v>
@@ -1312,13 +1312,13 @@
         <v>33</v>
       </c>
       <c r="H7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" t="s">
+        <v>128</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I7" t="s">
-        <v>130</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M7" t="s">
         <v>39</v>
@@ -1383,13 +1383,13 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I8" t="s">
-        <v>130</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M8" t="s">
         <v>56</v>
@@ -1454,13 +1454,13 @@
         <v>33</v>
       </c>
       <c r="H9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" t="s">
+        <v>128</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I9" t="s">
-        <v>130</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M9" t="s">
         <v>60</v>
@@ -1525,13 +1525,13 @@
         <v>33</v>
       </c>
       <c r="H10" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" t="s">
+        <v>128</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I10" t="s">
-        <v>130</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M10" t="s">
         <v>63</v>
@@ -1596,13 +1596,13 @@
         <v>33</v>
       </c>
       <c r="H11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" t="s">
+        <v>128</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I11" t="s">
-        <v>130</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M11" t="s">
         <v>66</v>
@@ -1667,13 +1667,13 @@
         <v>33</v>
       </c>
       <c r="H12" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I12" t="s">
-        <v>130</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M12" t="s">
         <v>69</v>
@@ -1738,13 +1738,13 @@
         <v>33</v>
       </c>
       <c r="H13" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" t="s">
+        <v>128</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I13" t="s">
-        <v>130</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M13" t="s">
         <v>72</v>
@@ -1809,13 +1809,13 @@
         <v>33</v>
       </c>
       <c r="H14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I14" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I14" t="s">
-        <v>130</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M14" t="s">
         <v>75</v>
@@ -1880,13 +1880,13 @@
         <v>33</v>
       </c>
       <c r="H15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I15" t="s">
+        <v>128</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I15" t="s">
-        <v>130</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M15" t="s">
         <v>78</v>
@@ -1951,13 +1951,13 @@
         <v>33</v>
       </c>
       <c r="H16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I16" t="s">
+        <v>128</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I16" t="s">
-        <v>130</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M16" t="s">
         <v>81</v>
@@ -2022,13 +2022,13 @@
         <v>33</v>
       </c>
       <c r="H17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" t="s">
+        <v>128</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I17" t="s">
-        <v>130</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M17" t="s">
         <v>88</v>
@@ -2078,13 +2078,13 @@
         <v>33</v>
       </c>
       <c r="H18" t="s">
+        <v>127</v>
+      </c>
+      <c r="I18" t="s">
+        <v>128</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="I18" t="s">
-        <v>130</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="M18" t="s">
         <v>91</v>
@@ -2149,13 +2149,13 @@
         <v>33</v>
       </c>
       <c r="H19" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I19" t="s">
-        <v>133</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M19" t="s">
         <v>34</v>
@@ -2205,13 +2205,13 @@
         <v>33</v>
       </c>
       <c r="H20" t="s">
+        <v>130</v>
+      </c>
+      <c r="I20" t="s">
+        <v>131</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I20" t="s">
-        <v>133</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M20" t="s">
         <v>49</v>
@@ -2244,7 +2244,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:34" ht="48" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -2261,13 +2261,13 @@
         <v>33</v>
       </c>
       <c r="H21" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I21" t="s">
-        <v>133</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M21" t="s">
         <v>52</v>
@@ -2303,10 +2303,10 @@
         <v>98</v>
       </c>
       <c r="AG21" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>52</v>
+        <v>136</v>
+      </c>
+      <c r="AH21" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:34" ht="32" x14ac:dyDescent="0.2">
@@ -2326,13 +2326,13 @@
         <v>33</v>
       </c>
       <c r="H22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I22" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I22" t="s">
-        <v>133</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M22" t="s">
         <v>54</v>
@@ -2382,13 +2382,13 @@
         <v>33</v>
       </c>
       <c r="H23" t="s">
+        <v>130</v>
+      </c>
+      <c r="I23" t="s">
+        <v>131</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I23" t="s">
-        <v>133</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M23" t="s">
         <v>39</v>
@@ -2453,13 +2453,13 @@
         <v>33</v>
       </c>
       <c r="H24" t="s">
+        <v>130</v>
+      </c>
+      <c r="I24" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I24" t="s">
-        <v>133</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M24" t="s">
         <v>56</v>
@@ -2524,13 +2524,13 @@
         <v>33</v>
       </c>
       <c r="H25" t="s">
+        <v>130</v>
+      </c>
+      <c r="I25" t="s">
+        <v>131</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I25" t="s">
-        <v>133</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M25" t="s">
         <v>60</v>
@@ -2595,13 +2595,13 @@
         <v>33</v>
       </c>
       <c r="H26" t="s">
+        <v>130</v>
+      </c>
+      <c r="I26" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I26" t="s">
-        <v>133</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M26" t="s">
         <v>63</v>
@@ -2666,13 +2666,13 @@
         <v>33</v>
       </c>
       <c r="H27" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27" t="s">
+        <v>131</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I27" t="s">
-        <v>133</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M27" t="s">
         <v>66</v>
@@ -2737,13 +2737,13 @@
         <v>33</v>
       </c>
       <c r="H28" t="s">
+        <v>130</v>
+      </c>
+      <c r="I28" t="s">
+        <v>131</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I28" t="s">
-        <v>133</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M28" t="s">
         <v>69</v>
@@ -2808,13 +2808,13 @@
         <v>33</v>
       </c>
       <c r="H29" t="s">
+        <v>130</v>
+      </c>
+      <c r="I29" t="s">
+        <v>131</v>
+      </c>
+      <c r="L29" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I29" t="s">
-        <v>133</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M29" t="s">
         <v>72</v>
@@ -2879,13 +2879,13 @@
         <v>33</v>
       </c>
       <c r="H30" t="s">
+        <v>130</v>
+      </c>
+      <c r="I30" t="s">
+        <v>131</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I30" t="s">
-        <v>133</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M30" t="s">
         <v>75</v>
@@ -2950,13 +2950,13 @@
         <v>33</v>
       </c>
       <c r="H31" t="s">
+        <v>130</v>
+      </c>
+      <c r="I31" t="s">
+        <v>131</v>
+      </c>
+      <c r="L31" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I31" t="s">
-        <v>133</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M31" t="s">
         <v>78</v>
@@ -3021,13 +3021,13 @@
         <v>33</v>
       </c>
       <c r="H32" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" t="s">
+        <v>131</v>
+      </c>
+      <c r="L32" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I32" t="s">
-        <v>133</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M32" t="s">
         <v>81</v>
@@ -3092,13 +3092,13 @@
         <v>33</v>
       </c>
       <c r="H33" t="s">
+        <v>130</v>
+      </c>
+      <c r="I33" t="s">
+        <v>131</v>
+      </c>
+      <c r="L33" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I33" t="s">
-        <v>133</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M33" t="s">
         <v>88</v>
@@ -3148,13 +3148,13 @@
         <v>33</v>
       </c>
       <c r="H34" t="s">
+        <v>130</v>
+      </c>
+      <c r="I34" t="s">
+        <v>131</v>
+      </c>
+      <c r="L34" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I34" t="s">
-        <v>133</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="M34" t="s">
         <v>91</v>

</xml_diff>